<commit_message>
Merged Lavanya's Code on 14th september
</commit_message>
<xml_diff>
--- a/Config/LogicalValues.xlsx
+++ b/Config/LogicalValues.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usha\PycharmProjects\M2MAutomation2\Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="LogicalNames" sheetId="2" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Type</t>
   </si>
@@ -61,9 +66,6 @@
     <t>_adfp_portlet_field___adfpfp_f2036994902_adfpsep_f0_adfpsep_description</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>textarea</t>
   </si>
   <si>
@@ -85,16 +87,85 @@
     <t>p</t>
   </si>
   <si>
-    <t>dropdown</t>
-  </si>
-  <si>
-    <t>__ns2036994902_organisationInputTree</t>
-  </si>
-  <si>
-    <t>ServiceProfOrganisation</t>
-  </si>
-  <si>
-    <t>__ns2036994902_organisationInputTreeTreeOrganisationInput</t>
+    <t>__ns2036994902_name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>__ns2036994902_searchFiltersSearchBtnText</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>ServiceProf</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//*[@class='globaltable dataTable']</t>
+  </si>
+  <si>
+    <t>ServingNetworkCode</t>
+  </si>
+  <si>
+    <t>__ns2036994902_searchCode</t>
+  </si>
+  <si>
+    <t>GHLRtemp</t>
+  </si>
+  <si>
+    <t>__ns2036994902_searchGhlrNameList</t>
+  </si>
+  <si>
+    <t>__ns2036994902_serviceProfileInput</t>
+  </si>
+  <si>
+    <t>Service Profile</t>
+  </si>
+  <si>
+    <t>__ns2036994902_configurationAreaEditBtn</t>
+  </si>
+  <si>
+    <t>ConfigEdit</t>
+  </si>
+  <si>
+    <t>__ns2036994902_searchProvisioningProfile</t>
+  </si>
+  <si>
+    <t>Provisioning profile</t>
+  </si>
+  <si>
+    <t>Create provisioning profile</t>
+  </si>
+  <si>
+    <t>inputlist</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>fieldBlock__field fieldBlock__field--withClean</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>__ns2036993941_withdrawDateCalendar</t>
+  </si>
+  <si>
+    <t>Withdraw Date (UTC)</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Description1234</t>
   </si>
 </sst>
 </file>
@@ -110,12 +181,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,11 +207,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +222,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -192,7 +273,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,7 +308,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,10 +589,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -525,55 +606,181 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>